<commit_message>
latest progress on the CVA MC simulation, DF and HJM
</commit_message>
<xml_diff>
--- a/finalProject/docs/CVA/CVA/SOLUTIONS.XLSX
+++ b/finalProject/docs/CVA/CVA/SOLUTIONS.XLSX
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alonso\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="20730" windowHeight="11700" tabRatio="654" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="20730" windowHeight="11700" tabRatio="654" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CVA_STATIC" sheetId="7" r:id="rId1"/>
@@ -19,7 +14,7 @@
     <sheet name="BILATERAL" sheetId="13" r:id="rId5"/>
     <sheet name="CVA_1234" sheetId="10" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -679,7 +674,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -725,26 +720,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -842,11 +817,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="235201120"/>
-        <c:axId val="235201904"/>
+        <c:axId val="8534656"/>
+        <c:axId val="35169024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="235201120"/>
+        <c:axId val="8534656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -903,12 +878,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235201904"/>
+        <c:crossAx val="35169024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="235201904"/>
+        <c:axId val="35169024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -965,7 +940,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235201120"/>
+        <c:crossAx val="8534656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1017,7 +992,7 @@
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1054,7 +1029,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1063,26 +1037,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1136,16 +1090,16 @@
                 <c:formatCode>_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* "-"??_ ;_-@_ </c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3984.0670875130927</c:v>
+                  <c:v>5408.1247754316373</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1123.5948118711808</c:v>
+                  <c:v>-48.270118246542552</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-4033.0565071061219</c:v>
+                  <c:v>-2699.1027750296671</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-4460.8934294082956</c:v>
+                  <c:v>-2355.0013220712563</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="[$$-409]#,##0.00_ ;\-[$$-409]#,##0.00\ ">
                   <c:v>0</c:v>
@@ -1168,11 +1122,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="231962984"/>
-        <c:axId val="231963376"/>
+        <c:axId val="136056192"/>
+        <c:axId val="136062080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="231962984"/>
+        <c:axId val="136056192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1230,12 +1184,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="231963376"/>
+        <c:crossAx val="136062080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="231963376"/>
+        <c:axId val="136062080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000"/>
@@ -1294,7 +1248,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="231962984"/>
+        <c:crossAx val="136056192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1346,7 +1300,7 @@
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1383,7 +1337,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1392,26 +1345,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1490,10 +1423,10 @@
                 <c:formatCode>_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* "-"??_ ;_-@_ </c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5362.1260520972628</c:v>
+                  <c:v>5029.051074826496</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>644.31474671636875</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1578,13 +1511,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>474.43460791607367</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2343.3260620944029</c:v>
+                  <c:v>2873.3682569102666</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1015.2511048427311</c:v>
+                  <c:v>2160.1054925269145</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1607,11 +1540,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="231957888"/>
-        <c:axId val="231964160"/>
+        <c:axId val="136108288"/>
+        <c:axId val="141300480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="231957888"/>
+        <c:axId val="136108288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1620,7 +1553,6 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1687,12 +1619,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="231964160"/>
+        <c:crossAx val="141300480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="231964160"/>
+        <c:axId val="141300480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000"/>
@@ -1715,7 +1647,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1782,7 +1713,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="231957888"/>
+        <c:crossAx val="136108288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1875,7 +1806,7 @@
 <file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1912,7 +1843,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1921,26 +1851,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2016,16 +1926,16 @@
                 <c:formatCode>0.000%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4.9104338028825904E-2</c:v>
+                  <c:v>5.2303685513942773E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.5665452079496849E-2</c:v>
+                  <c:v>4.6061490770890841E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8620826689781805E-2</c:v>
+                  <c:v>3.9727880697804939E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.5413770829298981E-2</c:v>
+                  <c:v>3.5058731313591135E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2095,16 +2005,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4.9104338028825904E-2</c:v>
+                  <c:v>5.2303685513942773E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.2226566130167793E-2</c:v>
+                  <c:v>3.9819296027838909E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4531575910351711E-2</c:v>
+                  <c:v>2.7060660551633128E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5792603247850515E-2</c:v>
+                  <c:v>2.105128316094973E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2292,11 +2202,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="231961416"/>
-        <c:axId val="231957496"/>
+        <c:axId val="141341440"/>
+        <c:axId val="141343744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="231961416"/>
+        <c:axId val="141341440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2329,7 +2239,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2338,26 +2247,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2396,12 +2285,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="231957496"/>
+        <c:crossAx val="141343744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="231957496"/>
+        <c:axId val="141343744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2448,7 +2337,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2457,26 +2345,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.000%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2515,7 +2383,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="231961416"/>
+        <c:crossAx val="141341440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2610,7 +2478,7 @@
 <file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2647,7 +2515,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2656,26 +2523,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2729,16 +2576,16 @@
                 <c:formatCode>_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* "-"??_ ;_-@_ </c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5362.1260520972628</c:v>
+                  <c:v>5029.051074826496</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>644.31474671636875</c:v>
+                  <c:v>-474.43460791607367</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2343.3260620944029</c:v>
+                  <c:v>-2873.3682569102666</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1015.2511048427311</c:v>
+                  <c:v>-2160.1054925269145</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="[$$-409]#,##0.00_ ;\-[$$-409]#,##0.00\ ">
                   <c:v>0</c:v>
@@ -2761,11 +2608,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="231959456"/>
-        <c:axId val="231964944"/>
+        <c:axId val="141459456"/>
+        <c:axId val="141460992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="231959456"/>
+        <c:axId val="141459456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2823,12 +2670,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="231964944"/>
+        <c:crossAx val="141460992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="231964944"/>
+        <c:axId val="141460992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000"/>
@@ -2887,7 +2734,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="231959456"/>
+        <c:crossAx val="141459456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2939,7 +2786,7 @@
 <file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2985,26 +2832,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -3070,16 +2897,16 @@
                 <c:formatCode>_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* "-"??_ ;_-@_ </c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2814.2113325660939</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5363.4080890737732</c:v>
+                  <c:v>10519.887955530645</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8096.2226266907292</c:v>
+                  <c:v>13736.025970188248</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6039.7782992640086</c:v>
+                  <c:v>8472.8065890798116</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -3102,11 +2929,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="235202688"/>
-        <c:axId val="232868120"/>
+        <c:axId val="141538816"/>
+        <c:axId val="141540736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="235202688"/>
+        <c:axId val="141538816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3164,12 +2991,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="232868120"/>
+        <c:crossAx val="141540736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="232868120"/>
+        <c:axId val="141540736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3226,7 +3053,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235202688"/>
+        <c:crossAx val="141538816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3278,7 +3105,7 @@
 <file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3324,26 +3151,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -3409,16 +3216,16 @@
                 <c:formatCode>0.000%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.0093859071500439E-2</c:v>
+                  <c:v>9.1070376733692702E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9527673574235734E-2</c:v>
+                  <c:v>1.8062886947837347E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.9154322669879339E-2</c:v>
+                  <c:v>3.2566398307777494E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.8140328805007492E-2</c:v>
+                  <c:v>4.3272291372873237E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3488,16 +3295,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.0093859071500439E-2</c:v>
+                  <c:v>9.1070376733692702E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8961488076971027E-2</c:v>
+                  <c:v>2.7018736222305426E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.8407620861166546E-2</c:v>
+                  <c:v>6.1573421027657789E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.5098347210391955E-2</c:v>
+                  <c:v>7.5389970568160464E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3683,11 +3490,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="232870472"/>
-        <c:axId val="232871256"/>
+        <c:axId val="142637696"/>
+        <c:axId val="142652544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="232870472"/>
+        <c:axId val="142637696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3729,26 +3536,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -3787,12 +3574,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="232871256"/>
+        <c:crossAx val="142652544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="232871256"/>
+        <c:axId val="142652544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="7.0000000000000007E-2"/>
@@ -3849,26 +3636,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.000%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -3907,7 +3674,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="232870472"/>
+        <c:crossAx val="142637696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3991,7 +3758,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4091,16 +3858,16 @@
                 <c:formatCode>_-"€"\ * #,##0.00_-;\-"€"\ * #,##0.00_-;_-"€"\ * "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.3956125919477573</c:v>
+                  <c:v>2.3957323785665854</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.930709940169387</c:v>
+                  <c:v>3.9329713984742773</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.1272405517954218</c:v>
+                  <c:v>3.1290397494530708</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3589045955020622</c:v>
+                  <c:v>1.3599925893414302</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4121,11 +3888,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="235202296"/>
-        <c:axId val="235203472"/>
+        <c:axId val="98317056"/>
+        <c:axId val="98318592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="235202296"/>
+        <c:axId val="98317056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4168,7 +3935,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235203472"/>
+        <c:crossAx val="98318592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4176,7 +3943,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="235203472"/>
+        <c:axId val="98318592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4227,7 +3994,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235202296"/>
+        <c:crossAx val="98317056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4279,7 +4046,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4325,26 +4092,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -4410,16 +4157,16 @@
                 <c:formatCode>_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* "-"??_ ;_-@_ </c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>446.89096614119546</c:v>
+                  <c:v>337.54791414950864</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1325.4898808530374</c:v>
+                  <c:v>1205.9879234592347</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1066.5594424145281</c:v>
+                  <c:v>931.74528431424505</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1181.1534071568051</c:v>
+                  <c:v>729.05697752344406</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4442,11 +4189,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="235199944"/>
-        <c:axId val="235200336"/>
+        <c:axId val="131352832"/>
+        <c:axId val="131359104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="235199944"/>
+        <c:axId val="131352832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4504,12 +4251,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235200336"/>
+        <c:crossAx val="131359104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="235200336"/>
+        <c:axId val="131359104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1400"/>
@@ -4568,7 +4315,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235199944"/>
+        <c:crossAx val="131352832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4620,7 +4367,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4666,26 +4413,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -4751,16 +4478,16 @@
                 <c:formatCode>0.000%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.8526583071009303E-4</c:v>
+                  <c:v>4.2587010043829241E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.6611833122269098E-3</c:v>
+                  <c:v>2.7121646242425522E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.9209951598247875E-3</c:v>
+                  <c:v>3.3790465870382948E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.3520514193625126E-3</c:v>
+                  <c:v>4.2414407368491901E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4830,16 +4557,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.8526583071009303E-4</c:v>
+                  <c:v>4.2587010043829241E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.9371007937437268E-3</c:v>
+                  <c:v>4.998459148046812E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.4406188550205425E-3</c:v>
+                  <c:v>4.7128105126297802E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.6452201979756883E-3</c:v>
+                  <c:v>6.828623186281876E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4940,11 +4667,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="235198768"/>
-        <c:axId val="235204648"/>
+        <c:axId val="131416064"/>
+        <c:axId val="131418368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="235198768"/>
+        <c:axId val="131416064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4986,26 +4713,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -5044,12 +4751,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235204648"/>
+        <c:crossAx val="131418368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="235204648"/>
+        <c:axId val="131418368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0000000000000002E-2"/>
@@ -5106,26 +4813,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.000%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -5164,7 +4851,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235198768"/>
+        <c:crossAx val="131416064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5248,7 +4935,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5285,7 +4972,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5294,26 +4980,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -5379,16 +5045,16 @@
                 <c:formatCode>_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* "-"??_ ;_-@_ </c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5617.8018883601271</c:v>
+                  <c:v>3995.6400533857859</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7963.1464297293296</c:v>
+                  <c:v>6445.0554868341005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7786.7478160187857</c:v>
+                  <c:v>6028.2700645803579</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5601.1749863737514</c:v>
+                  <c:v>4615.2207380787177</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -5411,11 +5077,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="235205824"/>
-        <c:axId val="235203080"/>
+        <c:axId val="131443712"/>
+        <c:axId val="133960832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="235205824"/>
+        <c:axId val="131443712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5472,12 +5138,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235203080"/>
+        <c:crossAx val="133960832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="235203080"/>
+        <c:axId val="133960832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000"/>
@@ -5536,7 +5202,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235205824"/>
+        <c:crossAx val="131443712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5588,7 +5254,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5625,7 +5291,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5634,26 +5299,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -5729,16 +5374,16 @@
                 <c:formatCode>0.000%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.057025324068865E-2</c:v>
+                  <c:v>2.0152851002932071E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5642476266491257E-2</c:v>
+                  <c:v>2.5920870098839192E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0075560568813768E-2</c:v>
+                  <c:v>2.9206371201806434E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.5862362085164731E-2</c:v>
+                  <c:v>3.4180476557414068E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5808,16 +5453,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.057025324068865E-2</c:v>
+                  <c:v>2.0152851002932071E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0714699292293864E-2</c:v>
+                  <c:v>3.1688889194746314E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8941729173458783E-2</c:v>
+                  <c:v>3.5777373407740912E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.3222766634217628E-2</c:v>
+                  <c:v>4.9102792624236974E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6005,11 +5650,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="235199160"/>
-        <c:axId val="235203864"/>
+        <c:axId val="134005504"/>
+        <c:axId val="134007808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="235199160"/>
+        <c:axId val="134005504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -6042,7 +5687,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6051,26 +5695,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -6109,12 +5733,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235203864"/>
+        <c:crossAx val="134007808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="235203864"/>
+        <c:axId val="134007808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="7.0000000000000007E-2"/>
@@ -6162,7 +5786,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6171,26 +5794,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.000%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -6229,7 +5832,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235199160"/>
+        <c:crossAx val="134005504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6324,7 +5927,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6361,7 +5964,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6370,26 +5972,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -6443,16 +6025,16 @@
                 <c:formatCode>_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* "-"??_ ;_-@_ </c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5617.8018883601271</c:v>
+                  <c:v>3995.6400533857859</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7963.1464297293296</c:v>
+                  <c:v>6445.0554868341005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7786.7478160187857</c:v>
+                  <c:v>6028.2700645803579</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5601.1749863737514</c:v>
+                  <c:v>4615.2207380787177</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="[$$-409]#,##0.00_ ;\-[$$-409]#,##0.00\ ">
                   <c:v>0</c:v>
@@ -6475,11 +6057,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="229503392"/>
-        <c:axId val="231958280"/>
+        <c:axId val="134376832"/>
+        <c:axId val="134382720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="229503392"/>
+        <c:axId val="134376832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -6537,12 +6119,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="231958280"/>
+        <c:crossAx val="134382720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="231958280"/>
+        <c:axId val="134382720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000"/>
@@ -6601,7 +6183,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229503392"/>
+        <c:crossAx val="134376832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6653,7 +6235,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6690,7 +6272,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6699,26 +6280,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -6784,7 +6345,7 @@
                 <c:formatCode>_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* "-"??_ ;_-@_ </c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3984.0670875130927</c:v>
+                  <c:v>5408.1247754316373</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -6816,11 +6377,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="231959064"/>
-        <c:axId val="231960240"/>
+        <c:axId val="134393216"/>
+        <c:axId val="134465024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="231959064"/>
+        <c:axId val="134393216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6877,12 +6438,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="231960240"/>
+        <c:crossAx val="134465024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="231960240"/>
+        <c:axId val="134465024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000"/>
@@ -6941,7 +6502,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="231959064"/>
+        <c:crossAx val="134393216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6993,7 +6554,7 @@
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -7030,7 +6591,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7039,26 +6599,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -7134,16 +6674,16 @@
                 <c:formatCode>0.000%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5.069120868516587E-2</c:v>
+                  <c:v>5.2111782306370764E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.6300809568241015E-2</c:v>
+                  <c:v>4.6482216045188686E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.1455670480791268E-2</c:v>
+                  <c:v>4.0515186782980231E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.3976688770345854E-2</c:v>
+                  <c:v>3.5446415304853693E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7213,16 +6753,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5.069120868516587E-2</c:v>
+                  <c:v>5.2111782306370764E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.191041045131616E-2</c:v>
+                  <c:v>4.0852649784006607E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.1765392305891774E-2</c:v>
+                  <c:v>2.8581128258563321E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1539743639009614E-2</c:v>
+                  <c:v>2.0240100870474079E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7410,11 +6950,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="231958672"/>
-        <c:axId val="231961024"/>
+        <c:axId val="136147328"/>
+        <c:axId val="136149632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="231958672"/>
+        <c:axId val="136147328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -7447,7 +6987,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7456,26 +6995,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -7514,12 +7033,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="231961024"/>
+        <c:crossAx val="136149632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="231961024"/>
+        <c:axId val="136149632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -7566,7 +7085,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7575,26 +7093,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.000%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -7633,7 +7131,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="231958672"/>
+        <c:crossAx val="136147328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -16878,8 +16376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -17105,7 +16603,7 @@
         <v>0.99600798934399148</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="K7" s="23">
         <f>$B$3</f>
@@ -17313,20 +16811,20 @@
         <v>10</v>
       </c>
       <c r="B19" s="24">
-        <f t="shared" ref="B19:E20" si="5">E7</f>
-        <v>0.99990000499983334</v>
+        <f>(1+E7)/2</f>
+        <v>0.99995000249991661</v>
       </c>
       <c r="C19" s="24">
-        <f t="shared" si="5"/>
-        <v>0.99875078092458092</v>
+        <f>(F7+E7)/2</f>
+        <v>0.99932539296220713</v>
       </c>
       <c r="D19" s="24">
-        <f t="shared" si="5"/>
-        <v>0.99760287769738176</v>
+        <f t="shared" ref="D19:E19" si="5">(G7+F7)/2</f>
+        <v>0.99817682931098139</v>
       </c>
       <c r="E19" s="24">
         <f t="shared" si="5"/>
-        <v>0.99600798934399148</v>
+        <v>0.99680543352068662</v>
       </c>
       <c r="J19" s="8" t="s">
         <v>57</v>
@@ -17341,19 +16839,19 @@
         <v>33</v>
       </c>
       <c r="B20" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="B19:E20" si="6">E8</f>
         <v>7.4719451808615833E-3</v>
       </c>
       <c r="C20" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7.4161152160757693E-3</v>
       </c>
       <c r="D20" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7.3607024097263052E-3</v>
       </c>
       <c r="E20" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7.3057036448281876E-3</v>
       </c>
       <c r="J20" s="4" t="s">
@@ -17381,15 +16879,15 @@
         <v>0.6</v>
       </c>
       <c r="C21" s="31">
-        <f t="shared" ref="C21:E21" si="6">1-$B$10</f>
+        <f t="shared" ref="C21:E21" si="7">1-$B$10</f>
         <v>0.6</v>
       </c>
       <c r="D21" s="31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.6</v>
       </c>
       <c r="E21" s="31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.6</v>
       </c>
       <c r="J21" s="14">
@@ -17414,19 +16912,19 @@
       </c>
       <c r="B22" s="34">
         <f>B18*B19*B20*B21</f>
-        <v>2.3956125919477573</v>
+        <v>2.3957323785665854</v>
       </c>
       <c r="C22" s="32">
-        <f t="shared" ref="C22:E22" si="7">C18*C19*C20*C21</f>
-        <v>3.930709940169387</v>
+        <f t="shared" ref="C22:E22" si="8">C18*C19*C20*C21</f>
+        <v>3.9329713984742773</v>
       </c>
       <c r="D22" s="32">
-        <f t="shared" si="7"/>
-        <v>3.1272405517954218</v>
+        <f t="shared" si="8"/>
+        <v>3.1290397494530708</v>
       </c>
       <c r="E22" s="32">
-        <f t="shared" si="7"/>
-        <v>1.3589045955020622</v>
+        <f t="shared" si="8"/>
+        <v>1.3599925893414302</v>
       </c>
       <c r="J22" s="21">
         <f>MAX(J13,0)</f>
@@ -17455,7 +16953,7 @@
       </c>
       <c r="B23" s="35">
         <f>SUM(B22:E22)</f>
-        <v>10.812467679414629</v>
+        <v>10.817736115835364</v>
       </c>
     </row>
   </sheetData>
@@ -17469,8 +16967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -17595,19 +17093,19 @@
       </c>
       <c r="E5" s="38">
         <f ca="1">E10*0.9+E10*0.2*RAND()</f>
-        <v>3.8526583071009303E-4</v>
+        <v>4.2587010043829241E-4</v>
       </c>
       <c r="F5" s="38">
         <f ca="1">F10*0.9+F10*0.2*RAND()</f>
-        <v>2.6611833122269098E-3</v>
+        <v>2.7121646242425522E-3</v>
       </c>
       <c r="G5" s="38">
         <f ca="1">G10*0.9+G10*0.2*RAND()</f>
-        <v>2.9209951598247875E-3</v>
+        <v>3.3790465870382948E-3</v>
       </c>
       <c r="H5" s="38">
         <f ca="1">H10*0.9+H10*0.2*RAND()</f>
-        <v>4.3520514193625126E-3</v>
+        <v>4.2414407368491901E-3</v>
       </c>
       <c r="J5" s="17" t="s">
         <v>18</v>
@@ -17641,38 +17139,38 @@
       </c>
       <c r="E6" s="26">
         <f ca="1">E5</f>
-        <v>3.8526583071009303E-4</v>
+        <v>4.2587010043829241E-4</v>
       </c>
       <c r="F6" s="26">
         <f ca="1">(F5*F4-E5*E4)/(F4-E4)</f>
-        <v>4.9371007937437268E-3</v>
+        <v>4.998459148046812E-3</v>
       </c>
       <c r="G6" s="26">
         <f ca="1">(G5*G4-F5*F4)/(G4-F4)</f>
-        <v>3.4406188550205425E-3</v>
+        <v>4.7128105126297802E-3</v>
       </c>
       <c r="H6" s="27">
         <f ca="1">(H5*H4-G5*G4)/(H4-G4)</f>
-        <v>8.6452201979756883E-3</v>
+        <v>6.828623186281876E-3</v>
       </c>
       <c r="J6" s="17" t="s">
         <v>19</v>
       </c>
       <c r="K6" s="23">
         <f ca="1">E6</f>
-        <v>3.8526583071009303E-4</v>
+        <v>4.2587010043829241E-4</v>
       </c>
       <c r="L6" s="23">
         <f t="shared" ref="L6:N6" ca="1" si="1">F6</f>
-        <v>4.9371007937437268E-3</v>
+        <v>4.998459148046812E-3</v>
       </c>
       <c r="M6" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>3.4406188550205425E-3</v>
+        <v>4.7128105126297802E-3</v>
       </c>
       <c r="N6" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>8.6452201979756883E-3</v>
+        <v>6.828623186281876E-3</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -17687,19 +17185,19 @@
       </c>
       <c r="E7" s="28">
         <f ca="1">EXP(-E5*E4)</f>
-        <v>0.9999036881806036</v>
+        <v>0.99989353814235626</v>
       </c>
       <c r="F7" s="28">
         <f ca="1">EXP(-F5*F4)</f>
-        <v>0.99867029318846512</v>
+        <v>0.99864483675200821</v>
       </c>
       <c r="G7" s="28">
         <f ca="1">EXP(-G5*G4)</f>
-        <v>0.99781165156355234</v>
+        <v>0.9974689236487353</v>
       </c>
       <c r="H7" s="29">
         <f ca="1">EXP(-H5*H4)</f>
-        <v>0.99565740503311961</v>
+        <v>0.99576754146926061</v>
       </c>
       <c r="J7" s="17" t="s">
         <v>15</v>
@@ -17748,19 +17246,19 @@
       </c>
       <c r="K8" s="24">
         <f ca="1">E7</f>
-        <v>0.9999036881806036</v>
+        <v>0.99989353814235626</v>
       </c>
       <c r="L8" s="24">
         <f ca="1">F7</f>
-        <v>0.99867029318846512</v>
+        <v>0.99864483675200821</v>
       </c>
       <c r="M8" s="24">
         <f ca="1">G7</f>
-        <v>0.99781165156355234</v>
+        <v>0.9974689236487353</v>
       </c>
       <c r="N8" s="24">
         <f ca="1">H7</f>
-        <v>0.99565740503311961</v>
+        <v>0.99576754146926061</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -17817,19 +17315,19 @@
       </c>
       <c r="K10" s="19">
         <f ca="1">K5*(K6-K7)*K8*K9</f>
-        <v>-878.5989147118421</v>
+        <v>-868.44000930972618</v>
       </c>
       <c r="L10" s="19">
         <f t="shared" ref="L10:N10" ca="1" si="4">L5*(L6-L7)*L8*L9</f>
-        <v>258.93043843850944</v>
+        <v>274.24263914498971</v>
       </c>
       <c r="M10" s="19">
         <f t="shared" ca="1" si="4"/>
-        <v>-114.593964742277</v>
+        <v>202.68830679080097</v>
       </c>
       <c r="N10" s="19">
         <f t="shared" ca="1" si="4"/>
-        <v>1181.1534071568051</v>
+        <v>729.05697752344406</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -17841,7 +17339,7 @@
     <row r="13" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J13" s="19">
         <f ca="1">SUM(K10:N10)</f>
-        <v>446.89096614119546</v>
+        <v>337.54791414950864</v>
       </c>
       <c r="K13" s="18" t="s">
         <v>24</v>
@@ -17850,7 +17348,7 @@
     <row r="14" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K14" s="19">
         <f ca="1">SUM(L10:N10)</f>
-        <v>1325.4898808530374</v>
+        <v>1205.9879234592347</v>
       </c>
       <c r="L14" s="18" t="s">
         <v>25</v>
@@ -17859,7 +17357,7 @@
     <row r="15" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L15" s="19">
         <f ca="1">SUM(M10:N10)</f>
-        <v>1066.5594424145281</v>
+        <v>931.74528431424505</v>
       </c>
       <c r="M15" s="18" t="s">
         <v>26</v>
@@ -17875,7 +17373,7 @@
       <c r="E16" s="8"/>
       <c r="M16" s="19">
         <f ca="1">SUM(N10)</f>
-        <v>1181.1534071568051</v>
+        <v>729.05697752344406</v>
       </c>
       <c r="N16" s="18" t="s">
         <v>27</v>
@@ -17905,19 +17403,19 @@
       </c>
       <c r="B18" s="30">
         <f ca="1">(J22+K22)/2</f>
-        <v>886.1904234971164</v>
+        <v>771.76791880437167</v>
       </c>
       <c r="C18" s="30">
         <f ca="1">(K22+L22)/2</f>
-        <v>1196.0246616337827</v>
+        <v>1068.86660388674</v>
       </c>
       <c r="D18" s="30">
         <f ca="1">(L22+M22)/2</f>
-        <v>1123.8564247856666</v>
+        <v>830.4011309188445</v>
       </c>
       <c r="E18" s="30">
         <f ca="1">(M22+N22)/2</f>
-        <v>590.57670357840254</v>
+        <v>364.52848876172203</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -17926,19 +17424,19 @@
       </c>
       <c r="B19" s="24">
         <f t="shared" ref="B19:E20" ca="1" si="5">E7</f>
-        <v>0.9999036881806036</v>
+        <v>0.99989353814235626</v>
       </c>
       <c r="C19" s="24">
         <f t="shared" ca="1" si="5"/>
-        <v>0.99867029318846512</v>
+        <v>0.99864483675200821</v>
       </c>
       <c r="D19" s="24">
         <f t="shared" ca="1" si="5"/>
-        <v>0.99781165156355234</v>
+        <v>0.9974689236487353</v>
       </c>
       <c r="E19" s="24">
         <f t="shared" ca="1" si="5"/>
-        <v>0.99565740503311961</v>
+        <v>0.99576754146926061</v>
       </c>
       <c r="J19" s="8" t="s">
         <v>57</v>
@@ -18026,35 +17524,35 @@
       </c>
       <c r="B22" s="34">
         <f ca="1">B18*B19*B20*B21</f>
-        <v>3.9725571174484844</v>
+        <v>3.4595961947390719</v>
       </c>
       <c r="C22" s="32">
         <f t="shared" ref="C22:E22" ca="1" si="7">C18*C19*C20*C21</f>
-        <v>5.3148374298501313</v>
+        <v>4.7496574353990537</v>
       </c>
       <c r="D22" s="32">
         <f t="shared" ca="1" si="7"/>
-        <v>4.9525619161532317</v>
+        <v>3.6581188903751887</v>
       </c>
       <c r="E22" s="32">
         <f t="shared" ca="1" si="7"/>
-        <v>2.5775051457264175</v>
+        <v>1.5911192949688495</v>
       </c>
       <c r="J22" s="21">
         <f ca="1">MAX(J13,0)</f>
-        <v>446.89096614119546</v>
+        <v>337.54791414950864</v>
       </c>
       <c r="K22" s="21">
         <f ca="1">MAX(K14,0)</f>
-        <v>1325.4898808530374</v>
+        <v>1205.9879234592347</v>
       </c>
       <c r="L22" s="21">
         <f ca="1">MAX(L15,0)</f>
-        <v>1066.5594424145281</v>
+        <v>931.74528431424505</v>
       </c>
       <c r="M22" s="21">
         <f ca="1">MAX(M16,0)</f>
-        <v>1181.1534071568051</v>
+        <v>729.05697752344406</v>
       </c>
       <c r="N22" s="21">
         <f>MAX(N17,0)</f>
@@ -18067,7 +17565,7 @@
       </c>
       <c r="B23" s="35">
         <f ca="1">SUM(B22:E22)</f>
-        <v>16.817461609178263</v>
+        <v>13.458491815482164</v>
       </c>
     </row>
   </sheetData>
@@ -18207,19 +17705,19 @@
       </c>
       <c r="E5" s="38">
         <f ca="1">E10*0.95+E10*0.1*RAND()</f>
-        <v>2.057025324068865E-2</v>
+        <v>2.0152851002932071E-2</v>
       </c>
       <c r="F5" s="38">
         <f t="shared" ref="F5:H5" ca="1" si="0">F10*0.95+F10*0.1*RAND()</f>
-        <v>2.5642476266491257E-2</v>
+        <v>2.5920870098839192E-2</v>
       </c>
       <c r="G5" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>3.0075560568813768E-2</v>
+        <v>2.9206371201806434E-2</v>
       </c>
       <c r="H5" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5862362085164731E-2</v>
+        <v>3.4180476557414068E-2</v>
       </c>
       <c r="J5" s="17" t="s">
         <v>18</v>
@@ -18253,38 +17751,38 @@
       </c>
       <c r="E6" s="26">
         <f ca="1">E5</f>
-        <v>2.057025324068865E-2</v>
+        <v>2.0152851002932071E-2</v>
       </c>
       <c r="F6" s="26">
         <f ca="1">(F5*F4-E5*E4)/(F4-E4)</f>
-        <v>3.0714699292293864E-2</v>
+        <v>3.1688889194746314E-2</v>
       </c>
       <c r="G6" s="26">
         <f ca="1">(G5*G4-F5*F4)/(G4-F4)</f>
-        <v>3.8941729173458783E-2</v>
+        <v>3.5777373407740912E-2</v>
       </c>
       <c r="H6" s="27">
         <f ca="1">(H5*H4-G5*G4)/(H4-G4)</f>
-        <v>5.3222766634217628E-2</v>
+        <v>4.9102792624236974E-2</v>
       </c>
       <c r="J6" s="17" t="s">
         <v>19</v>
       </c>
       <c r="K6" s="23">
         <f ca="1">E6</f>
-        <v>2.057025324068865E-2</v>
+        <v>2.0152851002932071E-2</v>
       </c>
       <c r="L6" s="23">
         <f t="shared" ref="L6:N6" ca="1" si="2">F6</f>
-        <v>3.0714699292293864E-2</v>
+        <v>3.1688889194746314E-2</v>
       </c>
       <c r="M6" s="23">
         <f t="shared" ca="1" si="2"/>
-        <v>3.8941729173458783E-2</v>
+        <v>3.5777373407740912E-2</v>
       </c>
       <c r="N6" s="23">
         <f t="shared" ca="1" si="2"/>
-        <v>5.3222766634217628E-2</v>
+        <v>4.9102792624236974E-2</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -18299,19 +17797,19 @@
       </c>
       <c r="E7" s="28">
         <f ca="1">EXP(-E5*E4)</f>
-        <v>0.99487063703097023</v>
+        <v>0.99497445775529514</v>
       </c>
       <c r="F7" s="28">
         <f ca="1">EXP(-F5*F4)</f>
-        <v>0.98726060379538128</v>
+        <v>0.98712318972790203</v>
       </c>
       <c r="G7" s="28">
         <f ca="1">EXP(-G5*G4)</f>
-        <v>0.97769582918361841</v>
+        <v>0.97833338908531831</v>
       </c>
       <c r="H7" s="29">
         <f ca="1">EXP(-H5*H4)</f>
-        <v>0.96477307369927057</v>
+        <v>0.96639707688038912</v>
       </c>
       <c r="J7" s="17" t="s">
         <v>15</v>
@@ -18360,19 +17858,19 @@
       </c>
       <c r="K8" s="24">
         <f ca="1">E7</f>
-        <v>0.99487063703097023</v>
+        <v>0.99497445775529514</v>
       </c>
       <c r="L8" s="24">
         <f ca="1">F7</f>
-        <v>0.98726060379538128</v>
+        <v>0.98712318972790203</v>
       </c>
       <c r="M8" s="24">
         <f ca="1">G7</f>
-        <v>0.97769582918361841</v>
+        <v>0.97833338908531831</v>
       </c>
       <c r="N8" s="24">
         <f ca="1">H7</f>
-        <v>0.96477307369927057</v>
+        <v>0.96639707688038912</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -18429,19 +17927,19 @@
       </c>
       <c r="K10" s="19">
         <f ca="1">K5*(K6-K7)*K8*K9</f>
-        <v>-2345.344541369202</v>
+        <v>-2449.4154334483151</v>
       </c>
       <c r="L10" s="19">
         <f t="shared" ref="L10:N10" ca="1" si="5">L5*(L6-L7)*L8*L9</f>
-        <v>176.39861371054332</v>
+        <v>416.78542225374269</v>
       </c>
       <c r="M10" s="19">
         <f t="shared" ca="1" si="5"/>
-        <v>2185.5728296450343</v>
+        <v>1413.0493265016405</v>
       </c>
       <c r="N10" s="19">
         <f t="shared" ca="1" si="5"/>
-        <v>5601.1749863737514</v>
+        <v>4615.2207380787177</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -18473,7 +17971,7 @@
     <row r="13" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J13" s="19">
         <f ca="1">SUM(K10:N10)</f>
-        <v>5617.8018883601271</v>
+        <v>3995.6400533857859</v>
       </c>
       <c r="K13" s="18" t="s">
         <v>24</v>
@@ -18482,7 +17980,7 @@
     <row r="14" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K14" s="19">
         <f ca="1">SUM(L10:N10)</f>
-        <v>7963.1464297293296</v>
+        <v>6445.0554868341005</v>
       </c>
       <c r="L14" s="18" t="s">
         <v>25</v>
@@ -18491,7 +17989,7 @@
     <row r="15" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L15" s="19">
         <f ca="1">SUM(M10:N10)</f>
-        <v>7786.7478160187857</v>
+        <v>6028.2700645803579</v>
       </c>
       <c r="M15" s="18" t="s">
         <v>26</v>
@@ -18507,7 +18005,7 @@
       <c r="E16" s="8"/>
       <c r="M16" s="19">
         <f ca="1">SUM(N10)</f>
-        <v>5601.1749863737514</v>
+        <v>4615.2207380787177</v>
       </c>
       <c r="N16" s="18" t="s">
         <v>27</v>
@@ -18529,19 +18027,19 @@
       </c>
       <c r="J17" s="40">
         <f ca="1">J13</f>
-        <v>5617.8018883601271</v>
+        <v>3995.6400533857859</v>
       </c>
       <c r="K17" s="40">
         <f ca="1">K14</f>
-        <v>7963.1464297293296</v>
+        <v>6445.0554868341005</v>
       </c>
       <c r="L17" s="40">
         <f ca="1">L15</f>
-        <v>7786.7478160187857</v>
+        <v>6028.2700645803579</v>
       </c>
       <c r="M17" s="40">
         <f ca="1">M16</f>
-        <v>5601.1749863737514</v>
+        <v>4615.2207380787177</v>
       </c>
       <c r="N17" s="20">
         <v>0</v>
@@ -18553,19 +18051,19 @@
       </c>
       <c r="B18" s="30">
         <f ca="1">(J22+K22)/2</f>
-        <v>6790.4741590447284</v>
+        <v>5220.3477701099437</v>
       </c>
       <c r="C18" s="30">
         <f ca="1">(K22+L22)/2</f>
-        <v>7874.9471228740576</v>
+        <v>6236.6627757072292</v>
       </c>
       <c r="D18" s="30">
         <f ca="1">(L22+M22)/2</f>
-        <v>6693.9614011962685</v>
+        <v>5321.7454013295373</v>
       </c>
       <c r="E18" s="30">
         <f ca="1">(M22+N22)/2</f>
-        <v>2800.5874931868757</v>
+        <v>2307.6103690393588</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -18574,19 +18072,19 @@
       </c>
       <c r="B19" s="24">
         <f t="shared" ref="B19:E20" ca="1" si="7">E7</f>
-        <v>0.99487063703097023</v>
+        <v>0.99497445775529514</v>
       </c>
       <c r="C19" s="24">
         <f t="shared" ca="1" si="7"/>
-        <v>0.98726060379538128</v>
+        <v>0.98712318972790203</v>
       </c>
       <c r="D19" s="24">
         <f t="shared" ca="1" si="7"/>
-        <v>0.97769582918361841</v>
+        <v>0.97833338908531831</v>
       </c>
       <c r="E19" s="24">
         <f t="shared" ca="1" si="7"/>
-        <v>0.96477307369927057</v>
+        <v>0.96639707688038912</v>
       </c>
       <c r="J19" s="8" t="s">
         <v>57</v>
@@ -18674,35 +18172,35 @@
       </c>
       <c r="B22" s="34">
         <f ca="1">B18*B19*B20*B21</f>
-        <v>30.286678074131949</v>
+        <v>23.286075178073624</v>
       </c>
       <c r="C22" s="32">
         <f t="shared" ref="C22:E22" ca="1" si="9">C18*C19*C20*C21</f>
-        <v>34.594509085717618</v>
+        <v>27.393740358059258</v>
       </c>
       <c r="D22" s="32">
         <f t="shared" ca="1" si="9"/>
-        <v>28.90396857693268</v>
+        <v>22.993838635458847</v>
       </c>
       <c r="E22" s="32">
         <f t="shared" ca="1" si="9"/>
-        <v>11.843706063616496</v>
+        <v>9.7753291778557703</v>
       </c>
       <c r="J22" s="21">
         <f ca="1">MAX(J13,0)</f>
-        <v>5617.8018883601271</v>
+        <v>3995.6400533857859</v>
       </c>
       <c r="K22" s="21">
         <f ca="1">MAX(K14,0)</f>
-        <v>7963.1464297293296</v>
+        <v>6445.0554868341005</v>
       </c>
       <c r="L22" s="21">
         <f ca="1">MAX(L15,0)</f>
-        <v>7786.7478160187857</v>
+        <v>6028.2700645803579</v>
       </c>
       <c r="M22" s="21">
         <f ca="1">MAX(M16,0)</f>
-        <v>5601.1749863737514</v>
+        <v>4615.2207380787177</v>
       </c>
       <c r="N22" s="21">
         <f>MAX(N17,0)</f>
@@ -18715,7 +18213,7 @@
       </c>
       <c r="B23" s="35">
         <f ca="1">SUM(B22:E22)</f>
-        <v>105.62886180039874</v>
+        <v>83.448983349447488</v>
       </c>
     </row>
   </sheetData>
@@ -18856,19 +18354,19 @@
       </c>
       <c r="E5" s="38">
         <f ca="1">E10*0.95+E10*0.1*RAND()</f>
-        <v>5.069120868516587E-2</v>
+        <v>5.2111782306370764E-2</v>
       </c>
       <c r="F5" s="38">
         <f t="shared" ref="F5:H5" ca="1" si="0">F10*0.95+F10*0.1*RAND()</f>
-        <v>4.6300809568241015E-2</v>
+        <v>4.6482216045188686E-2</v>
       </c>
       <c r="G5" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1455670480791268E-2</v>
+        <v>4.0515186782980231E-2</v>
       </c>
       <c r="H5" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3976688770345854E-2</v>
+        <v>3.5446415304853693E-2</v>
       </c>
       <c r="J5" s="17" t="s">
         <v>18</v>
@@ -18902,38 +18400,38 @@
       </c>
       <c r="E6" s="26">
         <f ca="1">E5</f>
-        <v>5.069120868516587E-2</v>
+        <v>5.2111782306370764E-2</v>
       </c>
       <c r="F6" s="26">
         <f ca="1">(F5*F4-E5*E4)/(F4-E4)</f>
-        <v>4.191041045131616E-2</v>
+        <v>4.0852649784006607E-2</v>
       </c>
       <c r="G6" s="26">
         <f ca="1">(G5*G4-F5*F4)/(G4-F4)</f>
-        <v>3.1765392305891774E-2</v>
+        <v>2.8581128258563321E-2</v>
       </c>
       <c r="H6" s="27">
         <f ca="1">(H5*H4-G5*G4)/(H4-G4)</f>
-        <v>1.1539743639009614E-2</v>
+        <v>2.0240100870474079E-2</v>
       </c>
       <c r="J6" s="17" t="s">
         <v>19</v>
       </c>
       <c r="K6" s="23">
         <f ca="1">E6</f>
-        <v>5.069120868516587E-2</v>
+        <v>5.2111782306370764E-2</v>
       </c>
       <c r="L6" s="23">
         <f t="shared" ref="L6:N6" ca="1" si="2">F6</f>
-        <v>4.191041045131616E-2</v>
+        <v>4.0852649784006607E-2</v>
       </c>
       <c r="M6" s="23">
         <f t="shared" ca="1" si="2"/>
-        <v>3.1765392305891774E-2</v>
+        <v>2.8581128258563321E-2</v>
       </c>
       <c r="N6" s="23">
         <f t="shared" ca="1" si="2"/>
-        <v>1.1539743639009614E-2</v>
+        <v>2.0240100870474079E-2</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -18948,19 +18446,19 @@
       </c>
       <c r="E7" s="28">
         <f ca="1">EXP(-E5*E4)</f>
-        <v>0.98740715964961567</v>
+        <v>0.98705655077041965</v>
       </c>
       <c r="F7" s="28">
         <f ca="1">EXP(-F5*F4)</f>
-        <v>0.97711550987344198</v>
+        <v>0.97702688635161439</v>
       </c>
       <c r="G7" s="28">
         <f ca="1">EXP(-G5*G4)</f>
-        <v>0.96938662499960337</v>
+        <v>0.97007063544726269</v>
       </c>
       <c r="H7" s="29">
         <f ca="1">EXP(-H5*H4)</f>
-        <v>0.96659403687045442</v>
+        <v>0.96517445142310554</v>
       </c>
       <c r="J7" s="17" t="s">
         <v>15</v>
@@ -19009,19 +18507,19 @@
       </c>
       <c r="K8" s="24">
         <f ca="1">E7</f>
-        <v>0.98740715964961567</v>
+        <v>0.98705655077041965</v>
       </c>
       <c r="L8" s="24">
         <f ca="1">F7</f>
-        <v>0.97711550987344198</v>
+        <v>0.97702688635161439</v>
       </c>
       <c r="M8" s="24">
         <f ca="1">G7</f>
-        <v>0.96938662499960337</v>
+        <v>0.97007063544726269</v>
       </c>
       <c r="N8" s="24">
         <f ca="1">H7</f>
-        <v>0.96659403687045442</v>
+        <v>0.96517445142310554</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -19078,19 +18576,19 @@
       </c>
       <c r="K10" s="19">
         <f ca="1">K5*(K6-K7)*K8*K9</f>
-        <v>5107.6618993842731</v>
+        <v>5456.3948936781808</v>
       </c>
       <c r="L10" s="19">
         <f t="shared" ref="L10:N10" ca="1" si="5">L5*(L6-L7)*L8*L9</f>
-        <v>2909.4616952349411</v>
+        <v>2650.8326567831241</v>
       </c>
       <c r="M10" s="19">
         <f t="shared" ca="1" si="5"/>
-        <v>427.83692230217378</v>
+        <v>-344.10145295841062</v>
       </c>
       <c r="N10" s="19">
         <f t="shared" ca="1" si="5"/>
-        <v>-4460.8934294082956</v>
+        <v>-2355.0013220712563</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -19122,7 +18620,7 @@
     <row r="13" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J13" s="19">
         <f ca="1">SUM(K10:N10)</f>
-        <v>3984.0670875130927</v>
+        <v>5408.1247754316373</v>
       </c>
       <c r="K13" s="18" t="s">
         <v>24</v>
@@ -19131,7 +18629,7 @@
     <row r="14" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K14" s="19">
         <f ca="1">SUM(L10:N10)</f>
-        <v>-1123.5948118711808</v>
+        <v>-48.270118246542552</v>
       </c>
       <c r="L14" s="18" t="s">
         <v>25</v>
@@ -19140,7 +18638,7 @@
     <row r="15" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L15" s="19">
         <f ca="1">SUM(M10:N10)</f>
-        <v>-4033.0565071061219</v>
+        <v>-2699.1027750296671</v>
       </c>
       <c r="M15" s="18" t="s">
         <v>26</v>
@@ -19156,7 +18654,7 @@
       <c r="E16" s="8"/>
       <c r="M16" s="19">
         <f ca="1">SUM(N10)</f>
-        <v>-4460.8934294082956</v>
+        <v>-2355.0013220712563</v>
       </c>
       <c r="N16" s="18" t="s">
         <v>27</v>
@@ -19178,19 +18676,19 @@
       </c>
       <c r="J17" s="40">
         <f ca="1">J13</f>
-        <v>3984.0670875130927</v>
+        <v>5408.1247754316373</v>
       </c>
       <c r="K17" s="40">
         <f ca="1">K14</f>
-        <v>-1123.5948118711808</v>
+        <v>-48.270118246542552</v>
       </c>
       <c r="L17" s="40">
         <f ca="1">L15</f>
-        <v>-4033.0565071061219</v>
+        <v>-2699.1027750296671</v>
       </c>
       <c r="M17" s="40">
         <f ca="1">M16</f>
-        <v>-4460.8934294082956</v>
+        <v>-2355.0013220712563</v>
       </c>
       <c r="N17" s="20">
         <v>0</v>
@@ -19202,7 +18700,7 @@
       </c>
       <c r="B18" s="30">
         <f ca="1">(J22+K22)/2</f>
-        <v>1992.0335437565464</v>
+        <v>2704.0623877158187</v>
       </c>
       <c r="C18" s="30">
         <f ca="1">(K22+L22)/2</f>
@@ -19223,19 +18721,19 @@
       </c>
       <c r="B19" s="24">
         <f t="shared" ref="B19:E20" ca="1" si="7">E7</f>
-        <v>0.98740715964961567</v>
+        <v>0.98705655077041965</v>
       </c>
       <c r="C19" s="24">
         <f t="shared" ca="1" si="7"/>
-        <v>0.97711550987344198</v>
+        <v>0.97702688635161439</v>
       </c>
       <c r="D19" s="24">
         <f t="shared" ca="1" si="7"/>
-        <v>0.96938662499960337</v>
+        <v>0.97007063544726269</v>
       </c>
       <c r="E19" s="24">
         <f t="shared" ca="1" si="7"/>
-        <v>0.96659403687045442</v>
+        <v>0.96517445142310554</v>
       </c>
       <c r="J19" s="8" t="s">
         <v>57</v>
@@ -19323,7 +18821,7 @@
       </c>
       <c r="B22" s="34">
         <f ca="1">B18*B19*B20*B21</f>
-        <v>8.8181573998299374</v>
+        <v>11.965853181376261</v>
       </c>
       <c r="C22" s="32">
         <f t="shared" ref="C22:E22" ca="1" si="9">C18*C19*C20*C21</f>
@@ -19339,7 +18837,7 @@
       </c>
       <c r="J22" s="21">
         <f ca="1">MAX(J13,0)</f>
-        <v>3984.0670875130927</v>
+        <v>5408.1247754316373</v>
       </c>
       <c r="K22" s="21">
         <f ca="1">MAX(K14,0)</f>
@@ -19364,7 +18862,7 @@
       </c>
       <c r="B23" s="35">
         <f ca="1">SUM(B22:E22)</f>
-        <v>8.8181573998299374</v>
+        <v>11.965853181376261</v>
       </c>
     </row>
   </sheetData>
@@ -19505,19 +19003,19 @@
       </c>
       <c r="E5" s="38">
         <f ca="1">E13*0.95+E13*0.1*RAND()</f>
-        <v>4.9104338028825904E-2</v>
+        <v>5.2303685513942773E-2</v>
       </c>
       <c r="F5" s="38">
         <f ca="1">F13*0.95+F13*0.1*RAND()</f>
-        <v>4.5665452079496849E-2</v>
+        <v>4.6061490770890841E-2</v>
       </c>
       <c r="G5" s="38">
         <f ca="1">G13*0.95+G13*0.1*RAND()</f>
-        <v>3.8620826689781805E-2</v>
+        <v>3.9727880697804939E-2</v>
       </c>
       <c r="H5" s="45">
         <f ca="1">H13*0.95+H13*0.1*RAND()</f>
-        <v>3.5413770829298981E-2</v>
+        <v>3.5058731313591135E-2</v>
       </c>
       <c r="J5" s="17" t="s">
         <v>18</v>
@@ -19551,38 +19049,38 @@
       </c>
       <c r="E6" s="26">
         <f ca="1">E5</f>
-        <v>4.9104338028825904E-2</v>
+        <v>5.2303685513942773E-2</v>
       </c>
       <c r="F6" s="26">
         <f ca="1">(F5*F4-E5*E4)/(F4-E4)</f>
-        <v>4.2226566130167793E-2</v>
+        <v>3.9819296027838909E-2</v>
       </c>
       <c r="G6" s="26">
         <f ca="1">(G5*G4-F5*F4)/(G4-F4)</f>
-        <v>2.4531575910351711E-2</v>
+        <v>2.7060660551633128E-2</v>
       </c>
       <c r="H6" s="27">
         <f ca="1">(H5*H4-G5*G4)/(H4-G4)</f>
-        <v>2.5792603247850515E-2</v>
+        <v>2.105128316094973E-2</v>
       </c>
       <c r="J6" s="17" t="s">
         <v>19</v>
       </c>
       <c r="K6" s="23">
         <f ca="1">E6</f>
-        <v>4.9104338028825904E-2</v>
+        <v>5.2303685513942773E-2</v>
       </c>
       <c r="L6" s="23">
         <f t="shared" ref="L6:N6" ca="1" si="1">F6</f>
-        <v>4.2226566130167793E-2</v>
+        <v>3.9819296027838909E-2</v>
       </c>
       <c r="M6" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4531575910351711E-2</v>
+        <v>2.7060660551633128E-2</v>
       </c>
       <c r="N6" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2.5792603247850515E-2</v>
+        <v>2.105128316094973E-2</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -19597,19 +19095,19 @@
       </c>
       <c r="E7" s="28">
         <f ca="1">EXP(-E5*E4)</f>
-        <v>0.98779895922325989</v>
+        <v>0.98700919707680745</v>
       </c>
       <c r="F7" s="28">
         <f ca="1">EXP(-F5*F4)</f>
-        <v>0.97742596801208992</v>
+        <v>0.97723243792342007</v>
       </c>
       <c r="G7" s="28">
         <f ca="1">EXP(-G5*G4)</f>
-        <v>0.97144986232191788</v>
+        <v>0.9706436114816871</v>
       </c>
       <c r="H7" s="29">
         <f ca="1">EXP(-H5*H4)</f>
-        <v>0.9652059595511715</v>
+        <v>0.96554870664839021</v>
       </c>
       <c r="J7" s="17" t="s">
         <v>15</v>
@@ -19658,19 +19156,19 @@
       </c>
       <c r="K8" s="24">
         <f ca="1">E7</f>
-        <v>0.98779895922325989</v>
+        <v>0.98700919707680745</v>
       </c>
       <c r="L8" s="24">
         <f ca="1">F7</f>
-        <v>0.97742596801208992</v>
+        <v>0.97723243792342007</v>
       </c>
       <c r="M8" s="24">
         <f ca="1">G7</f>
-        <v>0.97144986232191788</v>
+        <v>0.9706436114816871</v>
       </c>
       <c r="N8" s="24">
         <f ca="1">H7</f>
-        <v>0.9652059595511715</v>
+        <v>0.96554870664839021</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -19748,19 +19246,19 @@
       </c>
       <c r="K10" s="19">
         <f ca="1">K5*(K6-K7)*K8*K9</f>
-        <v>4717.8113053808938</v>
+        <v>5503.4856827425701</v>
       </c>
       <c r="L10" s="19">
         <f t="shared" ref="L10:N10" ca="1" si="6">L5*(L6-L7)*L8*L9</f>
-        <v>2987.6408088107719</v>
+        <v>2398.9336489941929</v>
       </c>
       <c r="M10" s="19">
         <f t="shared" ca="1" si="6"/>
-        <v>-1328.074957251672</v>
+        <v>-713.26276438335219</v>
       </c>
       <c r="N10" s="19">
         <f t="shared" ca="1" si="6"/>
-        <v>-1015.2511048427311</v>
+        <v>-2160.1054925269145</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -19823,7 +19321,7 @@
       </c>
       <c r="J13" s="19">
         <f ca="1">SUM(K10:N10)</f>
-        <v>5362.1260520972628</v>
+        <v>5029.051074826496</v>
       </c>
       <c r="K13" s="18" t="s">
         <v>24</v>
@@ -19857,7 +19355,7 @@
       </c>
       <c r="K14" s="19">
         <f ca="1">SUM(L10:N10)</f>
-        <v>644.31474671636875</v>
+        <v>-474.43460791607367</v>
       </c>
       <c r="L14" s="18" t="s">
         <v>25</v>
@@ -19866,7 +19364,7 @@
     <row r="15" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L15" s="19">
         <f ca="1">SUM(M10:N10)</f>
-        <v>-2343.3260620944029</v>
+        <v>-2873.3682569102666</v>
       </c>
       <c r="M15" s="18" t="s">
         <v>26</v>
@@ -19882,7 +19380,7 @@
       <c r="E16" s="8"/>
       <c r="M16" s="19">
         <f ca="1">SUM(N10)</f>
-        <v>-1015.2511048427311</v>
+        <v>-2160.1054925269145</v>
       </c>
       <c r="N16" s="18" t="s">
         <v>27</v>
@@ -19904,19 +19402,19 @@
       </c>
       <c r="J17" s="40">
         <f ca="1">J13</f>
-        <v>5362.1260520972628</v>
+        <v>5029.051074826496</v>
       </c>
       <c r="K17" s="40">
         <f ca="1">K14</f>
-        <v>644.31474671636875</v>
+        <v>-474.43460791607367</v>
       </c>
       <c r="L17" s="40">
         <f ca="1">L15</f>
-        <v>-2343.3260620944029</v>
+        <v>-2873.3682569102666</v>
       </c>
       <c r="M17" s="40">
         <f ca="1">M16</f>
-        <v>-1015.2511048427311</v>
+        <v>-2160.1054925269145</v>
       </c>
       <c r="N17" s="20">
         <v>0</v>
@@ -19928,11 +19426,11 @@
       </c>
       <c r="B18" s="30">
         <f ca="1">(J22+K22)/2</f>
-        <v>3003.2203994068159</v>
+        <v>2514.525537413248</v>
       </c>
       <c r="C18" s="30">
         <f ca="1">(K22+L22)/2</f>
-        <v>322.15737335818437</v>
+        <v>0</v>
       </c>
       <c r="D18" s="30">
         <f ca="1">(L22+M22)/2</f>
@@ -19949,19 +19447,19 @@
       </c>
       <c r="B19" s="24">
         <f t="shared" ref="B19:E19" ca="1" si="8">E7</f>
-        <v>0.98779895922325989</v>
+        <v>0.98700919707680745</v>
       </c>
       <c r="C19" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>0.97742596801208992</v>
+        <v>0.97723243792342007</v>
       </c>
       <c r="D19" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>0.97144986232191788</v>
+        <v>0.9706436114816871</v>
       </c>
       <c r="E19" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>0.9652059595511715</v>
+        <v>0.96554870664839021</v>
       </c>
       <c r="J19" s="8" t="s">
         <v>57</v>
@@ -20068,11 +19566,11 @@
       </c>
       <c r="J22" s="21">
         <f ca="1">MAX(J13,0)</f>
-        <v>5362.1260520972628</v>
+        <v>5029.051074826496</v>
       </c>
       <c r="K22" s="21">
         <f ca="1">MAX(K14,0)</f>
-        <v>644.31474671636875</v>
+        <v>0</v>
       </c>
       <c r="L22" s="21">
         <f ca="1">MAX(L15,0)</f>
@@ -20093,11 +19591,11 @@
       </c>
       <c r="B23" s="34">
         <f ca="1">B18*B19*B20*B21*B22</f>
-        <v>13.200290479882323</v>
+        <v>11.043455077273219</v>
       </c>
       <c r="C23" s="34">
         <f t="shared" ref="C23:E23" ca="1" si="10">C18*C19*C20*C21*C22</f>
-        <v>1.3802738186411969</v>
+        <v>0</v>
       </c>
       <c r="D23" s="34">
         <f t="shared" ca="1" si="10"/>
@@ -20116,15 +19614,15 @@
       </c>
       <c r="K23" s="21">
         <f ca="1">-MIN(K14,0)</f>
-        <v>0</v>
+        <v>474.43460791607367</v>
       </c>
       <c r="L23" s="21">
         <f ca="1">-MIN(L15,0)</f>
-        <v>2343.3260620944029</v>
+        <v>2873.3682569102666</v>
       </c>
       <c r="M23" s="21">
         <f ca="1">-MIN(M16,0)</f>
-        <v>1015.2511048427311</v>
+        <v>2160.1054925269145</v>
       </c>
       <c r="N23" s="21">
         <f>MIN(N17,0)</f>
@@ -20137,7 +19635,7 @@
       </c>
       <c r="B24" s="35">
         <f ca="1">SUM(B23:E23)</f>
-        <v>14.58056429852352</v>
+        <v>11.043455077273219</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -20171,19 +19669,19 @@
       </c>
       <c r="B28" s="30">
         <f ca="1">(J23+K23)/2</f>
-        <v>0</v>
+        <v>237.21730395803684</v>
       </c>
       <c r="C28" s="30">
         <f ca="1">(K23+L23)/2</f>
-        <v>1171.6630310472015</v>
+        <v>1673.9014324131701</v>
       </c>
       <c r="D28" s="30">
         <f ca="1">(L23+M23)/2</f>
-        <v>1679.2885834685671</v>
+        <v>2516.7368747185906</v>
       </c>
       <c r="E28" s="30">
         <f ca="1">(M23+N23)/2</f>
-        <v>507.62555242136557</v>
+        <v>1080.0527462634573</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -20192,19 +19690,19 @@
       </c>
       <c r="B29" s="24">
         <f t="shared" ref="B29:E30" ca="1" si="11">B19</f>
-        <v>0.98779895922325989</v>
+        <v>0.98700919707680745</v>
       </c>
       <c r="C29" s="24">
         <f t="shared" ca="1" si="11"/>
-        <v>0.97742596801208992</v>
+        <v>0.97723243792342007</v>
       </c>
       <c r="D29" s="24">
         <f t="shared" ca="1" si="11"/>
-        <v>0.97144986232191788</v>
+        <v>0.9706436114816871</v>
       </c>
       <c r="E29" s="24">
         <f t="shared" ca="1" si="11"/>
-        <v>0.9652059595511715</v>
+        <v>0.96554870664839021</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -20276,19 +19774,19 @@
       </c>
       <c r="B33" s="34">
         <f ca="1">B28*B29*B30*B31*B32</f>
-        <v>0</v>
+        <v>1.0418262216208756</v>
       </c>
       <c r="C33" s="34">
         <f t="shared" ref="C33:E33" ca="1" si="13">C28*C29*C30*C31*C32</f>
-        <v>5.0199558966051372</v>
+        <v>7.1703615878312794</v>
       </c>
       <c r="D33" s="34">
         <f t="shared" ca="1" si="13"/>
-        <v>7.0444097711367668</v>
+        <v>10.548640630648709</v>
       </c>
       <c r="E33" s="34">
         <f t="shared" ca="1" si="13"/>
-        <v>2.0842410099363011</v>
+        <v>4.4361234059125456</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -20297,7 +19795,7 @@
       </c>
       <c r="B34" s="35">
         <f ca="1">SUM(B33:E33)</f>
-        <v>14.148606677678204</v>
+        <v>23.196951846013413</v>
       </c>
     </row>
   </sheetData>
@@ -20311,7 +19809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -20438,19 +19936,19 @@
       </c>
       <c r="E5" s="38">
         <f ca="1">E10*0.9+E10*0.2*RAND()</f>
-        <v>1.0093859071500439E-2</v>
+        <v>9.1070376733692702E-3</v>
       </c>
       <c r="F5" s="38">
         <f ca="1">F10*0.9+F10*0.2*RAND()</f>
-        <v>1.9527673574235734E-2</v>
+        <v>1.8062886947837347E-2</v>
       </c>
       <c r="G5" s="38">
         <f ca="1">G10*0.9+G10*0.2*RAND()</f>
-        <v>2.9154322669879339E-2</v>
+        <v>3.2566398307777494E-2</v>
       </c>
       <c r="H5" s="38">
         <f ca="1">H10*0.9+H10*0.2*RAND()</f>
-        <v>3.8140328805007492E-2</v>
+        <v>4.3272291372873237E-2</v>
       </c>
       <c r="J5" s="17" t="s">
         <v>18</v>
@@ -20484,38 +19982,38 @@
       </c>
       <c r="E6" s="26">
         <f ca="1">E5</f>
-        <v>1.0093859071500439E-2</v>
+        <v>9.1070376733692702E-3</v>
       </c>
       <c r="F6" s="26">
         <f ca="1">(F5*F4-E5*E4)/(F4-E4)</f>
-        <v>2.8961488076971027E-2</v>
+        <v>2.7018736222305426E-2</v>
       </c>
       <c r="G6" s="26">
         <f ca="1">(G5*G4-F5*F4)/(G4-F4)</f>
-        <v>4.8407620861166546E-2</v>
+        <v>6.1573421027657789E-2</v>
       </c>
       <c r="H6" s="27">
         <f ca="1">(H5*H4-G5*G4)/(H4-G4)</f>
-        <v>6.5098347210391955E-2</v>
+        <v>7.5389970568160464E-2</v>
       </c>
       <c r="J6" s="17" t="s">
         <v>19</v>
       </c>
       <c r="K6" s="23">
         <f ca="1">E6</f>
-        <v>1.0093859071500439E-2</v>
+        <v>9.1070376733692702E-3</v>
       </c>
       <c r="L6" s="23">
         <f t="shared" ref="L6:N6" ca="1" si="1">F6</f>
-        <v>2.8961488076971027E-2</v>
+        <v>2.7018736222305426E-2</v>
       </c>
       <c r="M6" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>4.8407620861166546E-2</v>
+        <v>6.1573421027657789E-2</v>
       </c>
       <c r="N6" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>6.5098347210391955E-2</v>
+        <v>7.5389970568160464E-2</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -20530,19 +20028,19 @@
       </c>
       <c r="E7" s="28">
         <f ca="1">EXP(-E5*E4)</f>
-        <v>0.9974797164928465</v>
+        <v>0.99772583043252017</v>
       </c>
       <c r="F7" s="28">
         <f ca="1">EXP(-F5*F4)</f>
-        <v>0.99028367471004919</v>
+        <v>0.99100921751049309</v>
       </c>
       <c r="G7" s="28">
         <f ca="1">EXP(-G5*G4)</f>
-        <v>0.97837158044321781</v>
+        <v>0.9758710729023139</v>
       </c>
       <c r="H7" s="29">
         <f ca="1">EXP(-H5*H4)</f>
-        <v>0.96257785401315077</v>
+        <v>0.95765059456733204</v>
       </c>
       <c r="J7" s="17" t="s">
         <v>15</v>
@@ -20591,19 +20089,19 @@
       </c>
       <c r="K8" s="24">
         <f ca="1">E7</f>
-        <v>0.9974797164928465</v>
+        <v>0.99772583043252017</v>
       </c>
       <c r="L8" s="24">
         <f ca="1">F7</f>
-        <v>0.99028367471004919</v>
+        <v>0.99100921751049309</v>
       </c>
       <c r="M8" s="24">
         <f ca="1">G7</f>
-        <v>0.97837158044321781</v>
+        <v>0.9758710729023139</v>
       </c>
       <c r="N8" s="24">
         <f ca="1">H7</f>
-        <v>0.96257785401315077</v>
+        <v>0.95765059456733204</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -20660,19 +20158,19 @@
       </c>
       <c r="K10" s="19">
         <f ca="1">K5*(K6-K7)*K8*K9</f>
-        <v>-7457.6922436887135</v>
+        <v>-7705.6766229645518</v>
       </c>
       <c r="L10" s="19">
         <f t="shared" ref="L10:N10" ca="1" si="4">L5*(L6-L7)*L8*L9</f>
-        <v>-2732.8145376169559</v>
+        <v>-3216.1380146576021</v>
       </c>
       <c r="M10" s="19">
         <f t="shared" ca="1" si="4"/>
-        <v>2056.4443274267205</v>
+        <v>5263.2193811084362</v>
       </c>
       <c r="N10" s="19">
         <f t="shared" ca="1" si="4"/>
-        <v>6039.7782992640086</v>
+        <v>8472.8065890798116</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -20704,7 +20202,7 @@
     <row r="13" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J13" s="19">
         <f ca="1">SUM(K10:N10)</f>
-        <v>-2094.2841546149411</v>
+        <v>2814.2113325660939</v>
       </c>
       <c r="K13" s="18" t="s">
         <v>24</v>
@@ -20713,7 +20211,7 @@
     <row r="14" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K14" s="19">
         <f ca="1">SUM(L10:N10)</f>
-        <v>5363.4080890737732</v>
+        <v>10519.887955530645</v>
       </c>
       <c r="L14" s="18" t="s">
         <v>25</v>
@@ -20722,7 +20220,7 @@
     <row r="15" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L15" s="19">
         <f ca="1">SUM(M10:N10)</f>
-        <v>8096.2226266907292</v>
+        <v>13736.025970188248</v>
       </c>
       <c r="M15" s="18" t="s">
         <v>26</v>
@@ -20738,7 +20236,7 @@
       <c r="E16" s="8"/>
       <c r="M16" s="19">
         <f ca="1">SUM(N10)</f>
-        <v>6039.7782992640086</v>
+        <v>8472.8065890798116</v>
       </c>
       <c r="N16" s="18" t="s">
         <v>27</v>
@@ -20768,19 +20266,19 @@
       </c>
       <c r="B18" s="30">
         <f ca="1">(J22+K22)/2</f>
-        <v>2681.7040445368866</v>
+        <v>6667.0496440483694</v>
       </c>
       <c r="C18" s="30">
         <f ca="1">(K22+L22)/2</f>
-        <v>6729.8153578822512</v>
+        <v>12127.956962859447</v>
       </c>
       <c r="D18" s="30">
         <f ca="1">(L22+M22)/2</f>
-        <v>7068.0004629773684</v>
+        <v>11104.41627963403</v>
       </c>
       <c r="E18" s="30">
         <f ca="1">(M22+N22)/2</f>
-        <v>3019.8891496320043</v>
+        <v>4236.4032945399058</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -20789,19 +20287,19 @@
       </c>
       <c r="B19" s="24">
         <f t="shared" ref="B19:E20" ca="1" si="6">E7</f>
-        <v>0.9974797164928465</v>
+        <v>0.99772583043252017</v>
       </c>
       <c r="C19" s="24">
         <f t="shared" ca="1" si="6"/>
-        <v>0.99028367471004919</v>
+        <v>0.99100921751049309</v>
       </c>
       <c r="D19" s="24">
         <f t="shared" ca="1" si="6"/>
-        <v>0.97837158044321781</v>
+        <v>0.9758710729023139</v>
       </c>
       <c r="E19" s="24">
         <f t="shared" ca="1" si="6"/>
-        <v>0.96257785401315077</v>
+        <v>0.95765059456733204</v>
       </c>
       <c r="J19" s="8" t="s">
         <v>57</v>
@@ -20889,35 +20387,35 @@
       </c>
       <c r="B22" s="34">
         <f ca="1">B18*B19*B20*B21</f>
-        <v>11.992227189806675</v>
+        <v>29.821523889047434</v>
       </c>
       <c r="C22" s="32">
         <f t="shared" ref="C22:E22" ca="1" si="8">C18*C19*C20*C21</f>
-        <v>29.654491897033775</v>
+        <v>53.480204568575822</v>
       </c>
       <c r="D22" s="32">
         <f t="shared" ca="1" si="8"/>
-        <v>30.540131893170077</v>
+        <v>47.858456613398495</v>
       </c>
       <c r="E22" s="32">
         <f t="shared" ca="1" si="8"/>
-        <v>12.742075347735048</v>
+        <v>17.783518098398662</v>
       </c>
       <c r="J22" s="21">
         <f ca="1">MAX(J13,0)</f>
-        <v>0</v>
+        <v>2814.2113325660939</v>
       </c>
       <c r="K22" s="21">
         <f ca="1">MAX(K14,0)</f>
-        <v>5363.4080890737732</v>
+        <v>10519.887955530645</v>
       </c>
       <c r="L22" s="21">
         <f ca="1">MAX(L15,0)</f>
-        <v>8096.2226266907292</v>
+        <v>13736.025970188248</v>
       </c>
       <c r="M22" s="21">
         <f ca="1">MAX(M16,0)</f>
-        <v>6039.7782992640086</v>
+        <v>8472.8065890798116</v>
       </c>
       <c r="N22" s="21">
         <f>MAX(N17,0)</f>
@@ -20930,7 +20428,7 @@
       </c>
       <c r="B23" s="35">
         <f ca="1">SUM(B22:E22)</f>
-        <v>84.928926327745572</v>
+        <v>148.94370316942042</v>
       </c>
     </row>
   </sheetData>

</xml_diff>